<commit_message>
Cambios en excel con datos de entrada para evitar problemas de formato.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davl3232/Documents/uni/tg/Ane-stent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7212999-0EB6-BB4C-9089-40FCA3D25AD8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FEE601-55BA-4044-8CA3-C1D4429B60FE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16560" xr2:uid="{AE6AF57C-1B68-D043-AD2D-BF947757FFBC}"/>
   </bookViews>
@@ -127,7 +127,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,8 +445,8 @@
   <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O63" sqref="O58:O63"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,7 +517,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>0</v>
       </c>
       <c r="C2" s="4">
@@ -559,12 +559,13 @@
       <c r="O2" s="4">
         <v>10</v>
       </c>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>0</v>
       </c>
       <c r="C3" s="4">
@@ -606,12 +607,13 @@
       <c r="O3" s="4">
         <v>10</v>
       </c>
+      <c r="P3" s="4"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>0</v>
       </c>
       <c r="C4" s="4">
@@ -653,12 +655,13 @@
       <c r="O4" s="4">
         <v>10</v>
       </c>
+      <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>0</v>
       </c>
       <c r="C5" s="4">
@@ -700,12 +703,13 @@
       <c r="O5" s="4">
         <v>10</v>
       </c>
+      <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>0</v>
       </c>
       <c r="C6" s="4">
@@ -747,12 +751,13 @@
       <c r="O6" s="4">
         <v>10</v>
       </c>
+      <c r="P6" s="4"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>0</v>
       </c>
       <c r="C7" s="4">
@@ -794,8 +799,10 @@
       <c r="O7" s="4">
         <v>10</v>
       </c>
+      <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -809,12 +816,13 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="4">
         <v>0</v>
       </c>
       <c r="C9" s="4">
@@ -856,12 +864,13 @@
       <c r="O9" s="4">
         <v>10</v>
       </c>
+      <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>0</v>
       </c>
       <c r="C10" s="4">
@@ -903,12 +912,13 @@
       <c r="O10" s="4">
         <v>10</v>
       </c>
+      <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="4">
         <v>0</v>
       </c>
       <c r="C11" s="4">
@@ -950,12 +960,13 @@
       <c r="O11" s="4">
         <v>10</v>
       </c>
+      <c r="P11" s="4"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="4">
         <v>0</v>
       </c>
       <c r="C12" s="4">
@@ -997,12 +1008,13 @@
       <c r="O12" s="4">
         <v>10</v>
       </c>
+      <c r="P12" s="4"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="4">
         <v>0</v>
       </c>
       <c r="C13" s="4">
@@ -1044,12 +1056,13 @@
       <c r="O13" s="4">
         <v>10</v>
       </c>
+      <c r="P13" s="4"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="4">
         <v>0</v>
       </c>
       <c r="C14" s="4">
@@ -1091,8 +1104,10 @@
       <c r="O14" s="4">
         <v>10</v>
       </c>
+      <c r="P14" s="4"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -1106,12 +1121,13 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="4">
         <v>0</v>
       </c>
       <c r="C16" s="4">
@@ -1153,12 +1169,13 @@
       <c r="O16" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P16" s="4"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="4">
         <v>0</v>
       </c>
       <c r="C17" s="4">
@@ -1200,12 +1217,13 @@
       <c r="O17" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P17" s="4"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="4">
         <v>0</v>
       </c>
       <c r="C18" s="4">
@@ -1247,12 +1265,13 @@
       <c r="O18" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P18" s="4"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="4">
         <v>0</v>
       </c>
       <c r="C19" s="4">
@@ -1294,12 +1313,13 @@
       <c r="O19" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P19" s="4"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="4">
         <v>0</v>
       </c>
       <c r="C20" s="4">
@@ -1341,12 +1361,13 @@
       <c r="O20" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P20" s="4"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="4">
         <v>0</v>
       </c>
       <c r="C21" s="4">
@@ -1388,8 +1409,10 @@
       <c r="O21" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P21" s="4"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -1403,12 +1426,13 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P22" s="4"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="4">
         <v>1</v>
       </c>
       <c r="C23" s="4">
@@ -1444,12 +1468,13 @@
       <c r="O23" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P23" s="4"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="4">
         <v>1</v>
       </c>
       <c r="C24" s="4">
@@ -1485,12 +1510,13 @@
       <c r="O24" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P24" s="4"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="4">
         <v>1</v>
       </c>
       <c r="C25" s="4">
@@ -1526,12 +1552,13 @@
       <c r="O25" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P25" s="4"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="4">
         <v>1</v>
       </c>
       <c r="C26" s="4">
@@ -1567,12 +1594,13 @@
       <c r="O26" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P26" s="4"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="4">
         <v>1</v>
       </c>
       <c r="C27" s="4">
@@ -1608,12 +1636,13 @@
       <c r="O27" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P27" s="4"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="4">
         <v>1</v>
       </c>
       <c r="C28" s="4">
@@ -1649,8 +1678,10 @@
       <c r="O28" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P28" s="4"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1664,12 +1695,13 @@
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P29" s="4"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="4">
         <v>1</v>
       </c>
       <c r="C30" s="4">
@@ -1705,12 +1737,13 @@
       <c r="O30" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P30" s="4"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="4">
         <v>1</v>
       </c>
       <c r="C31" s="4">
@@ -1746,12 +1779,13 @@
       <c r="O31" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P31" s="4"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="4">
         <v>1</v>
       </c>
       <c r="C32" s="4">
@@ -1787,12 +1821,13 @@
       <c r="O32" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P32" s="4"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="4">
         <v>1</v>
       </c>
       <c r="C33" s="4">
@@ -1828,12 +1863,13 @@
       <c r="O33" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P33" s="4"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="4">
         <v>1</v>
       </c>
       <c r="C34" s="4">
@@ -1869,12 +1905,13 @@
       <c r="O34" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P34" s="4"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="4">
         <v>1</v>
       </c>
       <c r="C35" s="4">
@@ -1910,8 +1947,10 @@
       <c r="O35" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P35" s="4"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -1925,12 +1964,13 @@
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P36" s="4"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="4">
         <v>1</v>
       </c>
       <c r="C37" s="4">
@@ -1966,12 +2006,13 @@
       <c r="O37" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P37" s="4"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="4">
         <v>1</v>
       </c>
       <c r="C38" s="4">
@@ -2007,12 +2048,13 @@
       <c r="O38" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P38" s="4"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="4">
         <v>1</v>
       </c>
       <c r="C39" s="4">
@@ -2048,12 +2090,13 @@
       <c r="O39" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P39" s="4"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="4">
         <v>1</v>
       </c>
       <c r="C40" s="4">
@@ -2089,12 +2132,13 @@
       <c r="O40" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P40" s="4"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="4">
         <v>1</v>
       </c>
       <c r="C41" s="4">
@@ -2130,12 +2174,13 @@
       <c r="O41" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P41" s="4"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="4">
         <v>1</v>
       </c>
       <c r="C42" s="4">
@@ -2171,8 +2216,10 @@
       <c r="O42" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P42" s="4"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B43" s="4"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -2186,12 +2233,13 @@
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P43" s="4"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="4">
         <v>1</v>
       </c>
       <c r="C44" s="4">
@@ -2227,12 +2275,13 @@
       <c r="O44" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P44" s="4"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="4">
         <v>0</v>
       </c>
       <c r="C45" s="4">
@@ -2274,12 +2323,13 @@
       <c r="O45" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P45" s="4"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="4">
         <v>1</v>
       </c>
       <c r="C46" s="4">
@@ -2315,12 +2365,13 @@
       <c r="O46" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P46" s="4"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="4">
         <v>0</v>
       </c>
       <c r="C47" s="4">
@@ -2362,12 +2413,13 @@
       <c r="O47" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P47" s="4"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>17</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="4">
         <v>1</v>
       </c>
       <c r="C48" s="4">
@@ -2403,12 +2455,13 @@
       <c r="O48" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P48" s="4"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="4">
         <v>0</v>
       </c>
       <c r="C49" s="4">
@@ -2450,12 +2503,30 @@
       <c r="O49" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P49" s="4"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="4">
         <v>1</v>
       </c>
       <c r="C51" s="4">
@@ -2491,12 +2562,13 @@
       <c r="O51" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P51" s="4"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="4">
         <v>1</v>
       </c>
       <c r="C52" s="4">
@@ -2532,12 +2604,13 @@
       <c r="O52" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P52" s="4"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="4">
         <v>1</v>
       </c>
       <c r="C53" s="4">
@@ -2573,12 +2646,13 @@
       <c r="O53" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P53" s="4"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>17</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="4">
         <v>1</v>
       </c>
       <c r="C54" s="4">
@@ -2614,12 +2688,13 @@
       <c r="O54" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P54" s="4"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="4">
         <v>1</v>
       </c>
       <c r="C55" s="4">
@@ -2655,12 +2730,13 @@
       <c r="O55" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P55" s="4"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>17</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="4">
         <v>1</v>
       </c>
       <c r="C56" s="4">
@@ -2696,12 +2772,30 @@
       <c r="O56" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P56" s="4"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="4">
         <v>1</v>
       </c>
       <c r="C58" s="4">
@@ -2737,12 +2831,13 @@
       <c r="O58" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P58" s="4"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>0</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="4">
         <v>0</v>
       </c>
       <c r="C59" s="4">
@@ -2773,23 +2868,24 @@
         <v>0</v>
       </c>
       <c r="L59" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M59" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="N59" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="O59" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P59" s="4"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>0</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B60" s="4">
         <v>1</v>
       </c>
       <c r="C60" s="4">
@@ -2825,12 +2921,13 @@
       <c r="O60" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P60" s="4"/>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="4">
         <v>0</v>
       </c>
       <c r="C61" s="4">
@@ -2861,23 +2958,24 @@
         <v>0</v>
       </c>
       <c r="L61" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M61" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="N61" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="O61" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P61" s="4"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>0</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="4">
         <v>1</v>
       </c>
       <c r="C62" s="4">
@@ -2913,12 +3011,13 @@
       <c r="O62" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P62" s="4"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>0</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="4">
         <v>0</v>
       </c>
       <c r="C63" s="4">
@@ -2949,17 +3048,18 @@
         <v>0</v>
       </c>
       <c r="L63" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="M63" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="N63" s="4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="O63" s="4">
         <v>10</v>
       </c>
+      <c r="P63" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Arreglado problema de ángulos en archivo de configuración.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davl3232/Documents/uni/tg/Ane-stent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E29459-2BA4-D548-BA64-87EDC976CD44}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AC5031-07A0-6D44-84CC-EEB521837F54}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16560" xr2:uid="{AE6AF57C-1B68-D043-AD2D-BF947757FFBC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="88">
   <si>
     <t>/Users/davl3232/Documents/uni/tg/Ane-stent/modelos/uvSphere.vtk</t>
   </si>
@@ -81,7 +81,22 @@
     <t>1</t>
   </si>
   <si>
-    <t>.1</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>/Users/davl3232/Documents/uni/tg/Ane-stent/modelos/cilindroRadio.vtk</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>0.5</t>
   </si>
   <si>
     <t>kVCF</t>
@@ -135,9 +150,6 @@
     <t>diterations</t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
     <t>1 si es rígido, 0 si es suave.</t>
   </si>
   <si>
@@ -201,12 +213,6 @@
     <t>Rigidez de anclado. [0,1]</t>
   </si>
   <si>
-    <t>Escala de tiempo. [-inf, inf]</t>
-  </si>
-  <si>
-    <t>Proporción máxima de volumen para la pose. [-inf, inf]</t>
-  </si>
-  <si>
     <t>Iteraciones del solucionador de velocidades. [entero_positivo]</t>
   </si>
   <si>
@@ -217,6 +223,72 @@
   </si>
   <si>
     <t>Iteraciones del solucionador de deriva. [entero_positivo]</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>Escala de tiempo. (0, inf]</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1,2,4,8,16,32</t>
+  </si>
+  <si>
+    <t>0,0.2,0.4,0.6,0.8,1</t>
+  </si>
+  <si>
+    <t>-10,-6.66,-3.33,3.33,6.66,10</t>
+  </si>
+  <si>
+    <t>0,1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Proporción máxima de volumen para la postura. [-inf, inf]</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>cilindroRadio.vtk</t>
+  </si>
+  <si>
+    <t>bunny.vtk</t>
+  </si>
+  <si>
+    <t>cilindroo.vtk</t>
+  </si>
+  <si>
+    <t>cuadrado.vtk</t>
+  </si>
+  <si>
+    <t>cubo.vtk</t>
+  </si>
+  <si>
+    <t>icoSphere.vtk</t>
+  </si>
+  <si>
+    <t>piso.vtk</t>
+  </si>
+  <si>
+    <t>uvSphere.vtk</t>
+  </si>
+  <si>
+    <t>uvSphereG.vtk</t>
+  </si>
+  <si>
+    <t>rgc.vtk</t>
+  </si>
+  <si>
+    <t>0   0</t>
   </si>
 </sst>
 </file>
@@ -587,11 +659,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E397AD-78F2-F64B-8231-A4D5CCE0A41D}">
-  <dimension ref="A1:AH9"/>
+  <dimension ref="A1:AH44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,55 +741,55 @@
         <v>13</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="AG1" s="2" t="s">
         <v>15</v>
@@ -726,91 +798,91 @@
     </row>
     <row r="2" spans="1:34" s="5" customFormat="1" ht="208" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AF2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG2" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="AH2" s="3"/>
     </row>
@@ -849,13 +921,13 @@
         <v>0</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="O4" s="1">
         <v>10</v>
@@ -888,31 +960,28 @@
         <v>1</v>
       </c>
       <c r="Y4" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="Z4" s="1">
         <v>1</v>
       </c>
-      <c r="AA4" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="AB4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="1">
-        <v>1</v>
+      <c r="AA4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="AF4" s="1">
         <v>0</v>
-      </c>
-      <c r="AG4" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
@@ -950,13 +1019,13 @@
         <v>0</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="O5" s="1">
         <v>10</v>
@@ -989,31 +1058,28 @@
         <v>1</v>
       </c>
       <c r="Y5" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="Z5" s="1">
         <v>1</v>
       </c>
-      <c r="AA5" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="AB5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="1" t="s">
-        <v>36</v>
+      <c r="AA5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
@@ -1051,13 +1117,13 @@
         <v>0</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="O6" s="1">
         <v>10</v>
@@ -1090,31 +1156,28 @@
         <v>1</v>
       </c>
       <c r="Y6" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="Z6" s="1">
         <v>1</v>
       </c>
-      <c r="AA6" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="AB6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="1" t="s">
-        <v>36</v>
+      <c r="AA6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
@@ -1152,13 +1215,13 @@
         <v>0</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="O7" s="1">
         <v>10</v>
@@ -1191,31 +1254,28 @@
         <v>1</v>
       </c>
       <c r="Y7" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="Z7" s="1">
         <v>1</v>
       </c>
-      <c r="AA7" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="AB7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="1" t="s">
-        <v>36</v>
+      <c r="AA7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
@@ -1253,13 +1313,13 @@
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="O8" s="1">
         <v>10</v>
@@ -1292,31 +1352,28 @@
         <v>1</v>
       </c>
       <c r="Y8" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="Z8" s="1">
         <v>1</v>
       </c>
-      <c r="AA8" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="AB8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="1" t="s">
-        <v>36</v>
+      <c r="AA8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
@@ -1354,13 +1411,13 @@
         <v>0</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="O9" s="1">
         <v>10</v>
@@ -1393,31 +1450,1270 @@
         <v>1</v>
       </c>
       <c r="Y9" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="Z9" s="1">
         <v>1</v>
       </c>
-      <c r="AA9" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="AB9" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC9" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="1" t="s">
-        <v>36</v>
+      <c r="AA9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="V10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="1">
+        <v>-15</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="1">
+        <v>-9</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="1">
+        <v>-3</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="1">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="1">
+        <v>9</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="1">
+        <v>15</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglado prolema con la fricción de los cuerpos rígidos.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davl3232/Documents/uni/tg/Ane-stent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AC5031-07A0-6D44-84CC-EEB521837F54}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC166B8-35F8-A048-B812-480E3258332D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16560" xr2:uid="{AE6AF57C-1B68-D043-AD2D-BF947757FFBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="91">
   <si>
     <t>/Users/davl3232/Documents/uni/tg/Ane-stent/modelos/uvSphere.vtk</t>
   </si>
@@ -289,6 +289,15 @@
   </si>
   <si>
     <t>0   0</t>
+  </si>
+  <si>
+    <t>/Users/davl3232/Documents/uni/tg/Ane-stent/modelos/cilindroo.vtk</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>0.1</t>
   </si>
 </sst>
 </file>
@@ -339,11 +348,11 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,11 +668,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E397AD-78F2-F64B-8231-A4D5CCE0A41D}">
-  <dimension ref="A1:AH44"/>
+  <dimension ref="A1:AH50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,28 +805,28 @@
       </c>
       <c r="AH1" s="2"/>
     </row>
-    <row r="2" spans="1:34" s="5" customFormat="1" ht="208" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" s="4" customFormat="1" ht="208" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
       <c r="L2" s="3" t="s">
         <v>46</v>
       </c>
@@ -2714,6 +2723,221 @@
       </c>
       <c r="K44" s="1" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N49" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N50" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>0</v>
+      </c>
+      <c r="R50" s="1">
+        <v>0</v>
+      </c>
+      <c r="S50" s="1">
+        <v>0</v>
+      </c>
+      <c r="T50" s="1">
+        <v>0</v>
+      </c>
+      <c r="U50" s="1">
+        <v>0</v>
+      </c>
+      <c r="V50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W50" s="1">
+        <v>0</v>
+      </c>
+      <c r="X50" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y50" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z50" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA50" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF50" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregado script de bash y cambios en el código necesarios para probar rendimiento con iteraciones.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davl3232/Documents/uni/tg/Ane-stent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC166B8-35F8-A048-B812-480E3258332D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A790559-4A18-8D44-9211-0BD3E82F8783}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16560" xr2:uid="{AE6AF57C-1B68-D043-AD2D-BF947757FFBC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="95">
   <si>
     <t>/Users/davl3232/Documents/uni/tg/Ane-stent/modelos/uvSphere.vtk</t>
   </si>
@@ -298,6 +298,18 @@
   </si>
   <si>
     <t>0.1</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>-5</t>
+  </si>
+  <si>
+    <t>-2.5</t>
+  </si>
+  <si>
+    <t>2.5</t>
   </si>
 </sst>
 </file>
@@ -668,11 +680,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E397AD-78F2-F64B-8231-A4D5CCE0A41D}">
-  <dimension ref="A1:AH50"/>
+  <dimension ref="A1:AH58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N49" sqref="N49"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="178" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A52" sqref="A52:AF56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2835,9 +2847,6 @@
       <c r="K49" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N49" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="O49" s="1" t="s">
         <v>20</v>
       </c>
@@ -2883,7 +2892,7 @@
         <v>90</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="O50" s="1" t="s">
         <v>20</v>
@@ -2938,6 +2947,594 @@
       </c>
       <c r="AF50" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>0</v>
+      </c>
+      <c r="R52" s="1">
+        <v>0</v>
+      </c>
+      <c r="S52" s="1">
+        <v>0</v>
+      </c>
+      <c r="T52" s="1">
+        <v>0</v>
+      </c>
+      <c r="U52" s="1">
+        <v>0</v>
+      </c>
+      <c r="V52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W52" s="1">
+        <v>0</v>
+      </c>
+      <c r="X52" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y52" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA52" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF52" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>0</v>
+      </c>
+      <c r="R53" s="1">
+        <v>0</v>
+      </c>
+      <c r="S53" s="1">
+        <v>0</v>
+      </c>
+      <c r="T53" s="1">
+        <v>0</v>
+      </c>
+      <c r="U53" s="1">
+        <v>0</v>
+      </c>
+      <c r="V53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W53" s="1">
+        <v>0</v>
+      </c>
+      <c r="X53" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y53" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z53" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF53" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q54" s="1">
+        <v>0</v>
+      </c>
+      <c r="R54" s="1">
+        <v>0</v>
+      </c>
+      <c r="S54" s="1">
+        <v>0</v>
+      </c>
+      <c r="T54" s="1">
+        <v>0</v>
+      </c>
+      <c r="U54" s="1">
+        <v>0</v>
+      </c>
+      <c r="V54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W54" s="1">
+        <v>0</v>
+      </c>
+      <c r="X54" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y54" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z54" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD54" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE54" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF54" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q55" s="1">
+        <v>0</v>
+      </c>
+      <c r="R55" s="1">
+        <v>0</v>
+      </c>
+      <c r="S55" s="1">
+        <v>0</v>
+      </c>
+      <c r="T55" s="1">
+        <v>0</v>
+      </c>
+      <c r="U55" s="1">
+        <v>0</v>
+      </c>
+      <c r="V55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W55" s="1">
+        <v>0</v>
+      </c>
+      <c r="X55" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y55" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z55" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF55" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>0</v>
+      </c>
+      <c r="R56" s="1">
+        <v>0</v>
+      </c>
+      <c r="S56" s="1">
+        <v>0</v>
+      </c>
+      <c r="T56" s="1">
+        <v>0</v>
+      </c>
+      <c r="U56" s="1">
+        <v>0</v>
+      </c>
+      <c r="V56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W56" s="1">
+        <v>0</v>
+      </c>
+      <c r="X56" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y56" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z56" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA56" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD56" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE56" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF56" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q58" s="1">
+        <v>0</v>
+      </c>
+      <c r="R58" s="1">
+        <v>0</v>
+      </c>
+      <c r="S58" s="1">
+        <v>0</v>
+      </c>
+      <c r="T58" s="1">
+        <v>0</v>
+      </c>
+      <c r="U58" s="1">
+        <v>0</v>
+      </c>
+      <c r="V58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W58" s="1">
+        <v>0</v>
+      </c>
+      <c r="X58" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y58" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z58" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA58" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD58" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE58" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF58" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en excel de pruebas.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davl3232/Documents/uni/tg/Ane-stent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A790559-4A18-8D44-9211-0BD3E82F8783}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A6CCDE-5D40-AC47-9DDE-280182EE1843}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16560" xr2:uid="{AE6AF57C-1B68-D043-AD2D-BF947757FFBC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="95">
   <si>
     <t>/Users/davl3232/Documents/uni/tg/Ane-stent/modelos/uvSphere.vtk</t>
   </si>
@@ -680,11 +680,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E397AD-78F2-F64B-8231-A4D5CCE0A41D}">
-  <dimension ref="A1:AH58"/>
+  <dimension ref="A1:AH62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="178" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A52" sqref="A52:AF56"/>
+      <selection pane="bottomLeft" activeCell="AF62" sqref="A62:AF62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3528,12 +3528,404 @@
         <v>17</v>
       </c>
       <c r="AD58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF58" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J59" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AE58" s="1" t="s">
+      <c r="K59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>0</v>
+      </c>
+      <c r="R59" s="1">
+        <v>0</v>
+      </c>
+      <c r="S59" s="1">
+        <v>0</v>
+      </c>
+      <c r="T59" s="1">
+        <v>0</v>
+      </c>
+      <c r="U59" s="1">
+        <v>0</v>
+      </c>
+      <c r="V59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W59" s="1">
+        <v>0</v>
+      </c>
+      <c r="X59" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y59" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z59" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA59" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE59" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF59" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J60" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AF58" s="1" t="s">
+      <c r="K60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N60" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>0</v>
+      </c>
+      <c r="R60" s="1">
+        <v>0</v>
+      </c>
+      <c r="S60" s="1">
+        <v>0</v>
+      </c>
+      <c r="T60" s="1">
+        <v>0</v>
+      </c>
+      <c r="U60" s="1">
+        <v>0</v>
+      </c>
+      <c r="V60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W60" s="1">
+        <v>0</v>
+      </c>
+      <c r="X60" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y60" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z60" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA60" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD60" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE60" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF60" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O61" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q61" s="1">
+        <v>0</v>
+      </c>
+      <c r="R61" s="1">
+        <v>0</v>
+      </c>
+      <c r="S61" s="1">
+        <v>0</v>
+      </c>
+      <c r="T61" s="1">
+        <v>0</v>
+      </c>
+      <c r="U61" s="1">
+        <v>0</v>
+      </c>
+      <c r="V61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W61" s="1">
+        <v>0</v>
+      </c>
+      <c r="X61" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y61" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z61" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA61" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC61" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD61" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE61" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF61" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>0</v>
+      </c>
+      <c r="R62" s="1">
+        <v>0</v>
+      </c>
+      <c r="S62" s="1">
+        <v>0</v>
+      </c>
+      <c r="T62" s="1">
+        <v>0</v>
+      </c>
+      <c r="U62" s="1">
+        <v>0</v>
+      </c>
+      <c r="V62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W62" s="1">
+        <v>0</v>
+      </c>
+      <c r="X62" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y62" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z62" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA62" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC62" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD62" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE62" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF62" s="1" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>